<commit_message>
Major Update: Fatura Kes sekmesi ve Taslak Faturaları Oku özelliği eklendi
- Fatura Kes sekmesi eklendi (Fatura Taslak Oluştur sekmesinin yanına)
- Fatura İsimlendirme bölümü Fatura Kes sekmesine taşındı
- Taslak Faturaları Oku butonu eklendi (Chrome ile Zirve portalından taslak faturaları okur)
- Fatura Türü kolonu eklendi (E-FATURA, E-ARŞİV)
- E-fatura ve E-arşiv taslakları otomatik okunup tabloya yazılıyor
- Zebra görünümü tüm tablolara uygulandı
- Ürün kartları düzenleme özelliği eklendi
- Inline fiyat düzenleme özelliği eklendi
- KORUMA KURALI eklendi (mevcut kodları değiştirme, sadece ekleme)
- Kod temizleme ve optimizasyon yapıldı
- Backup sistemi eklendi
</commit_message>
<xml_diff>
--- a/test_fatura_zirve.xlsx
+++ b/test_fatura_zirve.xlsx
@@ -518,7 +518,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>YEDEK PARÇA (24V SELENOİD)</t>
+          <t>a (b)</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>650</v>
+        <v>150</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -542,10 +542,41 @@
         <v>20</v>
       </c>
       <c r="H2" t="n">
-        <v>350000</v>
-      </c>
-    </row>
-    <row r="3"/>
+        <v>30</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>d (e)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>C62</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+    </row>
     <row r="4"/>
     <row r="5"/>
   </sheetData>

</xml_diff>